<commit_message>
Author       : Sourabh Description  :burnt hours excel sheet
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/Sourabh.xlsx
+++ b/TeamDetails/TasksBreakDown/Sourabh.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sourabh mishra\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship_2017_Prep.git\trunk\TeamDetails\TasksBreakDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="31">
   <si>
     <t>Story ID</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Understanding the concept of CSS</t>
   </si>
   <si>
-    <t>Make block diagram of the entire code journey(work flow)</t>
-  </si>
-  <si>
     <t>Technical understanding(bootstrap)</t>
   </si>
   <si>
@@ -93,10 +90,40 @@
     <t>Task-5</t>
   </si>
   <si>
-    <t>Task-6</t>
+    <t>Task-7</t>
   </si>
   <si>
-    <t>Task-7</t>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Task-8</t>
+  </si>
+  <si>
+    <t>Understanding angularjs and javascript</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Implementing angularjs and javascript</t>
+  </si>
+  <si>
+    <t>Task-9</t>
+  </si>
+  <si>
+    <t>Task-10</t>
+  </si>
+  <si>
+    <t>Task-11</t>
+  </si>
+  <si>
+    <t>Understanding backeng</t>
+  </si>
+  <si>
+    <t>implementing backend</t>
   </si>
 </sst>
 </file>
@@ -198,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -227,6 +254,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2836,10 +2866,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2850,9 +2880,10 @@
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2874,17 +2905,19 @@
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="8">
-        <f>SUM(E2:E8)</f>
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
@@ -2899,12 +2932,15 @@
         <f>E2-F2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="9"/>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>11</v>
@@ -2916,18 +2952,21 @@
         <v>1</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G45" si="0">E3-F3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G3:G5" si="0">E3-F3</f>
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="9"/>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="6">
         <v>4</v>
@@ -2936,12 +2975,15 @@
         <v>4</v>
       </c>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="9"/>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
@@ -2949,17 +2991,22 @@
       <c r="E5" s="6">
         <v>3</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="6">
+        <v>3</v>
+      </c>
       <c r="G5" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="9"/>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>9</v>
@@ -2969,83 +3016,115 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="9"/>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="10"/>
       <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="7">
-        <v>6</v>
+        <v>23</v>
+      </c>
+      <c r="E8" s="6">
+        <v>2</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="6">
+        <v>4</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="6">
+        <v>2</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <f>E10-F10</f>
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="6">
+        <v>4</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <f>E11-F11</f>
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3053,11 +3132,11 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <f>E12-F12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3065,11 +3144,11 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <f>E13-F13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -3077,11 +3156,11 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <f>E14-F14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -3089,11 +3168,11 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <f>E15-F15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -3101,7 +3180,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2">
-        <f t="shared" si="0"/>
+        <f>E16-F16</f>
         <v>0</v>
       </c>
     </row>
@@ -3113,7 +3192,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2">
-        <f t="shared" si="0"/>
+        <f>E17-F17</f>
         <v>0</v>
       </c>
     </row>
@@ -3125,7 +3204,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2">
-        <f t="shared" si="0"/>
+        <f>E18-F18</f>
         <v>0</v>
       </c>
     </row>
@@ -3137,7 +3216,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2">
-        <f t="shared" si="0"/>
+        <f>E19-F19</f>
         <v>0</v>
       </c>
     </row>
@@ -3149,7 +3228,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2">
-        <f t="shared" si="0"/>
+        <f>E20-F20</f>
         <v>0</v>
       </c>
     </row>
@@ -3161,7 +3240,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2">
-        <f t="shared" si="0"/>
+        <f>E21-F21</f>
         <v>0</v>
       </c>
     </row>
@@ -3173,7 +3252,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2">
-        <f t="shared" si="0"/>
+        <f>E22-F22</f>
         <v>0</v>
       </c>
     </row>
@@ -3185,7 +3264,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2">
-        <f t="shared" si="0"/>
+        <f>E23-F23</f>
         <v>0</v>
       </c>
     </row>
@@ -3197,7 +3276,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2">
-        <f t="shared" si="0"/>
+        <f>E24-F24</f>
         <v>0</v>
       </c>
     </row>
@@ -3209,7 +3288,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2">
-        <f t="shared" si="0"/>
+        <f>E25-F25</f>
         <v>0</v>
       </c>
     </row>
@@ -3221,7 +3300,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2">
-        <f t="shared" si="0"/>
+        <f>E26-F26</f>
         <v>0</v>
       </c>
     </row>
@@ -3233,7 +3312,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2">
-        <f t="shared" si="0"/>
+        <f>E27-F27</f>
         <v>0</v>
       </c>
     </row>
@@ -3245,7 +3324,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2">
-        <f t="shared" si="0"/>
+        <f>E28-F28</f>
         <v>0</v>
       </c>
     </row>
@@ -3257,7 +3336,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2">
-        <f t="shared" si="0"/>
+        <f>E29-F29</f>
         <v>0</v>
       </c>
     </row>
@@ -3269,7 +3348,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2">
-        <f t="shared" si="0"/>
+        <f>E30-F30</f>
         <v>0</v>
       </c>
     </row>
@@ -3281,7 +3360,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2">
-        <f t="shared" si="0"/>
+        <f>E31-F31</f>
         <v>0</v>
       </c>
     </row>
@@ -3293,7 +3372,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2">
-        <f t="shared" si="0"/>
+        <f>E32-F32</f>
         <v>0</v>
       </c>
     </row>
@@ -3305,7 +3384,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2">
-        <f t="shared" si="0"/>
+        <f>E33-F33</f>
         <v>0</v>
       </c>
     </row>
@@ -3317,7 +3396,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2">
-        <f t="shared" si="0"/>
+        <f>E34-F34</f>
         <v>0</v>
       </c>
     </row>
@@ -3329,7 +3408,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2">
-        <f t="shared" si="0"/>
+        <f>E35-F35</f>
         <v>0</v>
       </c>
     </row>
@@ -3341,7 +3420,7 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2">
-        <f t="shared" si="0"/>
+        <f>E36-F36</f>
         <v>0</v>
       </c>
     </row>
@@ -3353,7 +3432,7 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2">
-        <f t="shared" si="0"/>
+        <f>E37-F37</f>
         <v>0</v>
       </c>
     </row>
@@ -3365,7 +3444,7 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2">
-        <f t="shared" si="0"/>
+        <f>E38-F38</f>
         <v>0</v>
       </c>
     </row>
@@ -3377,7 +3456,7 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2">
-        <f t="shared" si="0"/>
+        <f>E39-F39</f>
         <v>0</v>
       </c>
     </row>
@@ -3389,7 +3468,7 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2">
-        <f t="shared" si="0"/>
+        <f>E40-F40</f>
         <v>0</v>
       </c>
     </row>
@@ -3401,7 +3480,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2">
-        <f t="shared" si="0"/>
+        <f>E41-F41</f>
         <v>0</v>
       </c>
     </row>
@@ -3413,7 +3492,7 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2">
-        <f t="shared" si="0"/>
+        <f>E42-F42</f>
         <v>0</v>
       </c>
     </row>
@@ -3425,7 +3504,7 @@
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2">
-        <f t="shared" si="0"/>
+        <f>E43-F43</f>
         <v>0</v>
       </c>
     </row>
@@ -3437,21 +3516,13 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2">
-        <f t="shared" si="0"/>
+        <f>E44-F44</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>